<commit_message>
rename to UNS Mapper
</commit_message>
<xml_diff>
--- a/mount/node-red/template/template-en.xlsx
+++ b/mount/node-red/template/template-en.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -105,7 +105,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">按照不同协议，填不同值，例如：
+          <t xml:space="preserve">Protocol-Specific Value Formatting Guide​
 </t>
         </r>
         <r>
@@ -123,7 +123,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">：填数组下标 0,1,2,3..
+          <t xml:space="preserve">：Array index [0, 1, 2, 3...]
 .
 </t>
         </r>
@@ -142,7 +142,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">：格式ns=0;s=item1;
+          <t xml:space="preserve">：ns=&lt;NamespaceIndex&gt;;s=&lt;Identifier&gt;;
 </t>
         </r>
         <r>
@@ -160,7 +160,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">：填写地址：bacnet.device1._Statistics._FailedWrites
+          <t xml:space="preserve">：&lt;ProgID&gt;.&lt;Device&gt;.&lt;ItemPath&gt;
 </t>
         </r>
       </text>
@@ -242,6 +242,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>AttributeName(</t>
     </r>
     <r>
@@ -268,6 +275,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>AttributeType(</t>
     </r>
     <r>
@@ -294,6 +308,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>TagConfiguration(</t>
     </r>
     <r>
@@ -1296,7 +1317,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
merge from release 11
</commit_message>
<xml_diff>
--- a/mount/node-red/template/template-en.xlsx
+++ b/mount/node-red/template/template-en.xlsx
@@ -161,14 +161,7 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FilePath(</t>
+      <t>Path(</t>
     </r>
     <r>
       <rPr>
@@ -466,12 +459,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1017,13 +1010,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
-<customStorage xmlns="https://web.wps.cn/et/2018/main">
-  <book/>
-  <sheets/>
-</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1279,7 +1265,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
feat(installation):update to version: V1.1.0.0-M
</commit_message>
<xml_diff>
--- a/mount/node-red/template/template-en.xlsx
+++ b/mount/node-red/template/template-en.xlsx
@@ -161,6 +161,13 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Path(</t>
     </r>
     <r>
@@ -186,7 +193,7 @@
     </r>
   </si>
   <si>
-    <t>FileAlias</t>
+    <t>Alias</t>
   </si>
   <si>
     <r>
@@ -459,12 +466,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1265,7 +1272,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>

</xml_diff>